<commit_message>
gross rate analysis RMD
</commit_message>
<xml_diff>
--- a/misc/Methane play.xlsx
+++ b/misc/Methane play.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3x290/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/kendalynn_morris_pnnl_gov/Documents/Documents/methane/grossMethane/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D4C421-8A1E-C94D-820E-D9634EBC6B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="27520" windowHeight="17040" xr2:uid="{22BE8FC2-5F99-7940-A92B-BA3015306541}"/>
+    <workbookView xWindow="-16960" yWindow="2240" windowWidth="14400" windowHeight="7810" xr2:uid="{22BE8FC2-5F99-7940-A92B-BA3015306541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -76,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,7 +109,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,6 +641,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1956026112"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2574,13 +2575,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE41554-D013-A746-BB8A-30B3E3079C22}">
   <dimension ref="B2:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -2596,7 +2597,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -2612,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -2640,16 +2641,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B9)</f>
+        <f t="shared" ref="C9:C19" si="0">D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B9)</f>
         <v>1</v>
       </c>
       <c r="D9">
-        <f>D$3*EXP(-D$6*D$4*B9)</f>
+        <f t="shared" ref="D9:D19" si="1">D$3*EXP(-D$6*D$4*B9)</f>
         <v>0.1</v>
       </c>
       <c r="E9">
@@ -2657,20 +2658,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B10)</f>
+        <f t="shared" si="0"/>
         <v>1.3934693402873666</v>
       </c>
       <c r="D10" s="1">
-        <f>D$3*EXP(-D$6*D$4*B10)</f>
+        <f t="shared" si="1"/>
         <v>6.1262639418441615E-2</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" ref="E10:E19" si="0">D10/C10*100</f>
+        <f t="shared" ref="E10:E19" si="2">D10/C10*100</f>
         <v>4.3964110043359694</v>
       </c>
       <c r="F10" s="1">
@@ -2682,228 +2683,228 @@
         <v>0.60653065971263342</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B11)</f>
+        <f t="shared" si="0"/>
         <v>1.6321205588285577</v>
       </c>
       <c r="D11" s="1">
-        <f>D$3*EXP(-D$6*D$4*B11)</f>
+        <f t="shared" si="1"/>
         <v>3.7531109885139961E-2</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2995304900808087</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F19" si="1">C11-C10</f>
+        <f t="shared" ref="F11:F19" si="3">C11-C10</f>
         <v>0.23865121854119109</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G19" si="2">D$5-F11</f>
+        <f t="shared" ref="G11:G19" si="4">D$5-F11</f>
         <v>0.76134878145880891</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B12)</f>
+        <f t="shared" si="0"/>
         <v>1.7768698398515701</v>
       </c>
       <c r="D12" s="1">
-        <f>D$3*EXP(-D$6*D$4*B12)</f>
+        <f t="shared" si="1"/>
         <v>2.2992548518672384E-2</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2939917152622196</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14474928102301243</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.85525071897698757</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B13)</f>
+        <f t="shared" si="0"/>
         <v>1.8646647167633872</v>
       </c>
       <c r="D13" s="1">
-        <f>D$3*EXP(-D$6*D$4*B13)</f>
+        <f t="shared" si="1"/>
         <v>1.4085842092104501E-2</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.75540883921234692</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.7794876911817088E-2</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.91220512308818291</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>5</v>
       </c>
       <c r="C14" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B14)</f>
+        <f t="shared" si="0"/>
         <v>1.9179150013761013</v>
       </c>
       <c r="D14" s="1">
-        <f>D$3*EXP(-D$6*D$4*B14)</f>
+        <f t="shared" si="1"/>
         <v>8.6293586499370505E-3</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.44993436329271624</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.3250284612714083E-2</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.94674971538728592</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B15)</f>
+        <f t="shared" si="0"/>
         <v>1.9502129316321362</v>
       </c>
       <c r="D15" s="1">
-        <f>D$3*EXP(-D$6*D$4*B15)</f>
+        <f t="shared" si="1"/>
         <v>5.2865728738350371E-3</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27107670080982882</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.229793025603489E-2</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.96770206974396511</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B16)</f>
+        <f t="shared" si="0"/>
         <v>1.9698026165776814</v>
       </c>
       <c r="D16" s="1">
-        <f>D$3*EXP(-D$6*D$4*B16)</f>
+        <f t="shared" si="1"/>
         <v>3.2386940772907054E-3</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16441718830273389</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9589684945545249E-2</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.98041031505445475</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>8</v>
       </c>
       <c r="C17" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B17)</f>
+        <f t="shared" si="0"/>
         <v>1.9816843611112658</v>
       </c>
       <c r="D17" s="1">
-        <f>D$3*EXP(-D$6*D$4*B17)</f>
+        <f t="shared" si="1"/>
         <v>1.9841094744370287E-3</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.10012237636696103</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1881744533584371E-2</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.98811825546641563</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>9</v>
       </c>
       <c r="C18" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B18)</f>
+        <f t="shared" si="0"/>
         <v>1.9888910034617577</v>
       </c>
       <c r="D18" s="1">
-        <f>D$3*EXP(-D$6*D$4*B18)</f>
+        <f t="shared" si="1"/>
         <v>1.2155178329914937E-3</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.1115356793098666E-2</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2066423504919541E-3</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.99279335764950805</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>10</v>
       </c>
       <c r="C19" s="1">
-        <f>D$5/D$6-(D$5/D$6-D$2)*EXP(-D$6*B19)</f>
+        <f t="shared" si="0"/>
         <v>1.9932620530009146</v>
       </c>
       <c r="D19" s="1">
-        <f>D$3*EXP(-D$6*D$4*B19)</f>
+        <f t="shared" si="1"/>
         <v>7.4465830709243388E-4</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7358776081214656E-2</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3710495391569015E-3</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.9956289504608431</v>
       </c>
     </row>

</xml_diff>